<commit_message>
Fix bugs and add AlumnoE0
</commit_message>
<xml_diff>
--- a/public/assets/images/user-import/Plantilla_Usuarios_LIA.xlsx
+++ b/public/assets/images/user-import/Plantilla_Usuarios_LIA.xlsx
@@ -92,7 +92,7 @@
     <t>ProfesorSummit2021</t>
   </si>
   <si>
-    <t>Metropolitan</t>
+    <t>AlumnoE0</t>
   </si>
   <si>
     <t>Primaria - Segundo Grado</t>
@@ -126,7 +126,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -140,7 +140,7 @@
     </font>
     <font>
       <color rgb="FF586573"/>
-      <name val="Arial"/>
+      <name val="&quot;DM Sans&quot;"/>
     </font>
     <font>
       <color theme="1"/>
@@ -151,8 +151,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF1D1C1D"/>
+      <name val="Slack-Lato"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -165,6 +170,12 @@
         <bgColor rgb="FFF5F9FC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -172,7 +183,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -193,6 +204,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5624,7 +5638,7 @@
       <c r="B6" s="8">
         <v>6.0</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E6" s="3">
@@ -5638,7 +5652,7 @@
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="8">

</xml_diff>